<commit_message>
fix console admin signup
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>user</t>
   </si>
   <si>
+    <t>driver_id</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -80,9 +83,6 @@
   </si>
   <si>
     <t>user_id</t>
-  </si>
-  <si>
-    <t>driver_id</t>
   </si>
   <si>
     <t>brand_id</t>
@@ -1045,7 +1045,7 @@
   <dimension ref="B2:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:H28"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1054,164 +1054,167 @@
     <col min="4" max="4" width="11.9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="2:8">
       <c r="B23" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="2:8">
       <c r="B25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
         <v>23</v>
       </c>
       <c r="F25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="4:4">

</xml_diff>